<commit_message>
inicio del análisis exploratorio
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Docencia\Analítica3\Trabajos\datos_caso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/741792de0362012a/Escritorio/HR_T1_Analitica/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB35FA0B-ACC7-4365-A392-02C60593CAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -814,10 +814,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1178,17 +1178,17 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="99.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>78</v>
       </c>
@@ -1228,14 +1228,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1273,35 +1273,35 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -1339,28 +1339,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
@@ -1380,28 +1380,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
       <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
@@ -1430,28 +1430,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>48</v>
       </c>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>50</v>
       </c>
@@ -1507,28 +1507,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>55</v>
       </c>
@@ -1539,28 +1539,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
       <c r="C43" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>57</v>
       </c>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>59</v>
       </c>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>61</v>
       </c>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>65</v>
       </c>
@@ -1607,28 +1607,28 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
       <c r="C50" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
       <c r="C51" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
       <c r="C52" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>70</v>
       </c>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>72</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>74</v>
       </c>
@@ -1657,6 +1657,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B22:B25"/>
@@ -1666,13 +1673,6 @@
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>